<commit_message>
this version only writes org names to excel with their indices. Two columns but not quite right
</commit_message>
<xml_diff>
--- a/rgv-sheet.xlsx
+++ b/rgv-sheet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B329"/>
+  <dimension ref="A1:B317"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Contact: DionicioEmail: diongartist@yahoo.comPhone: 1.956.778.5854Address: 1221 W Campbell RdCity: Richardson</t>
+          <t>(TASO) Texas Association of Sports Officials Rio Grande Valley Basketball Chapter</t>
         </is>
       </c>
     </row>
@@ -454,7 +454,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Contact: Melissa GutierrezEmail: 911rgministries@gmail.comPhone: 1-956-331-7943Address: 15712 South Gaston CircleCity: Edinburg</t>
+          <t>9-1-1 Ministries</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Contact: Maricela MedranoEmail: medranom@awfc.orgPhone: 1-956-683-9917Address: 2917 N. 23rd StCity: McAllen</t>
+          <t>A World for Children</t>
         </is>
       </c>
     </row>
@@ -474,7 +474,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Contact: Mary Jo BecerraEmail: aimstrong03@gmail.comPhone: 1-956-378-6874Address: Address: PO Box 1454City: Edinburg</t>
+          <t>A.I.M. Strong, Inc.</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Contact: CarlosEmail: carlos.aactnow@gmail.comPhone: 1-956-664-2228Address: Address: 612 Nolana Ave. Suite 430City: McAllen</t>
+          <t>AACT Advocacy Alliance Center of Texas</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Contact: Peter PinonEmail: peterpinon@msn.comPhone: 1-956-454-5774Address: 101 North O. streetCity: Harlingen</t>
+          <t>Abundant Life Church</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Contact: Kathryn HearnEmail: info@accessclinics.orgPhone: 1-956-688-3700Address: 916 E. HackberryCity: McAllen</t>
+          <t>Access Esperanza Clinics</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Contact: GustavoEmail: gustavo.salinas@dfps.state.tx.usPhone: 1-956-316-8348Address: 2520 S. Veterans Blvd.City: Edinburg</t>
+          <t>Adopt-A-Beach Program, Texas General Land Office</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Contact: Virginia HaynieEmail: vhgause@gmail.comPhone: 1-956-358-3915Address: McAllen Creative Incubator – Studio 17City: McAllen</t>
+          <t>Adult Protective Services</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Contact: Diana GonzalezEmail: aurorahousefoundation@yahoo.comPhone: 1-956-973-9690Address: 2646 W. 18th StreetCity: Weslaco</t>
+          <t>Advocacy Alliance Center of Texas (AACT)</t>
         </is>
       </c>
     </row>
@@ -544,7 +544,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Contact: Joel N Pena, JrEmail: Joel.Pena@uhsrgv.comPhone: 1-956-388-2020Address: 301 W Expressway 83City: McAllen</t>
+          <t>Advocacy Resource Center for Housing (ARCH)</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Contact: Tomas Cantu JrEmail: tcantujr.rgv@avance.orgPhone: 1-956-354-2130Address: 811 E. Bowie Ave.City: Alamo</t>
+          <t>Affordable Homes of South Texas, Inc.</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Contact: DebraEmail: Debra_Franco@baylor.eduPhone: 1-956-802-0654Address: 200 S 10th St, Mcallen, TX 78501City: McAllen</t>
+          <t>Alton Recreation Center</t>
         </is>
       </c>
     </row>
@@ -574,7 +574,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Contact: Marissa CanoEmail: Hc0414@bcfs.netPhone: 1-956-630-0010Address: 211 N. 15th StCity: McAllen</t>
+          <t>Alzheimer’s Association</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Contact: GildaEmail: gbowen@bhsst.orgPhone: 1-956-787-0004Address: 5510 N. Cage Blvd, Ste. R, Pharr, TXCity: Pharr</t>
+          <t>Amara Hospice</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Contact: Martha L. GonzalezEmail: blessings@bigherotx.orgPhone: 1-956-455-3129Address: 814 Boca Chica Blvd.City: Brownsville</t>
+          <t>American Cancer Society, Rio Grande Valley</t>
         </is>
       </c>
     </row>
@@ -604,7 +604,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Contact: Marco CordovaEmail: marccordova@gmail.comPhone: 1-956-313-6235Address: 5617 E. Trenton Rd. Suite C Edinburg, TX 78539City: Edinburg</t>
+          <t>American Civil Liberties Union</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Contact: Ernest EspinozaEmail: eernest@BSAmail.orgPhone: 1-214-907-9759Address: 6912 W. Expressway 83City: Harlingen</t>
+          <t>American Foundation for Suicide Prevention: South Texas Chapter</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Contact: AlmaEmail: almadones@yahoo.comPhone: 1-956-428-7816Address: 1215 Rangerville Rd, Harlingen, TX 78552City: Harlingen</t>
+          <t>American Red Cross</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Contact: Jessica Soliz</t>
+          <t>Amigos Del Valle, Inc.</t>
         </is>
       </c>
     </row>
@@ -644,7 +644,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Email: jsoliz@bgcmcallen.netPhone: 1-956-682-5791Address: 2620 W. GalvestonCity: McAllen</t>
+          <t>Angels of Love</t>
         </is>
       </c>
     </row>
@@ -654,7 +654,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Contact: Cristina CastilloEmail: ccastillo@missiontexas.usPhone: 1-956-585-3606Address: 209 W. 18th StreetCity: Mission</t>
+          <t xml:space="preserve">Arise Support Center South Tower </t>
         </is>
       </c>
     </row>
@@ -664,7 +664,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Contact: Stephanie LealEmail: sleal@pharrkids.orgPhone: 1-956-781-5437Address: 1026 S. Fir StreetCity: Pharr</t>
+          <t>Arroyo Colorado Audubon Society</t>
         </is>
       </c>
     </row>
@@ -674,7 +674,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Contact: Ashley MartinezEmail: ronnierod9@hotmail.comPhone: 1-956-973-1610Address: 300 N Airport Dr Suite BCity: Weslaco</t>
+          <t>ArtsRGV</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Contact: Nathanial PenaEmail: npena@edinburgkids.comPhone: 1-956-383-2582Address: 702 Cullen StreetCity: Edinburg</t>
+          <t>Aurora House Foundation</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Contact: Iris GarciaEmail: irisbgc@gmail.comPhone: 1-956-295-8707Address: 900 N. Arroyo BlvdCity: Los Fresnos</t>
+          <t>Auxiliary to South Texas Health System, Inc.</t>
         </is>
       </c>
     </row>
@@ -704,7 +704,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Contact: Natalie or StephanieEmail: natalie832@gmail.com;  stephramirez84@gmail.comPhone: 1-832-446-7129 (Natalie); 1-832-373-1709 (Stephanie)City: Houston</t>
+          <t>AVANCE</t>
         </is>
       </c>
     </row>
@@ -714,7 +714,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Email: info@brownsvillecommunityfoundation.orgPhone: 1-956-572-3730Address: 549 E. Levee St. Brownsville, TX 78520City: Brownsville</t>
+          <t>Baylor Texas Hunger Initiative</t>
         </is>
       </c>
     </row>
@@ -724,7 +724,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Contact: PaulaEmail: psgomez.bchc@tachc.orgEmail: info@tachc.orgPhone: 1-956-548-7400Address: 191 E Price Rd Brownsville, TX 78521City: Brownsville</t>
+          <t>BCFS Health and Human Services</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Contact: Tara PutegnatEmail: info@brownsvillehistory.orgPhone: 1-956-372-1515Address: 1325 E. Washington StreetCity: Brownsville</t>
+          <t>Behavioral Health Solutions of South Texas</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Contact: Victor RiveraEmail: brownsvilleliteracy@yahoo.comPhone: 1-956-542-8080Address: 245 E. Levee St.City: Brownsville</t>
+          <t>BiG Heroes, INC.</t>
         </is>
       </c>
     </row>
@@ -754,7 +754,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Contact: Dee RamirezEmail: dramirez@brownsvillemfa.orgPhone: 1-956-542-0941Address: 660 E Ringgold StCity: Brownsville</t>
+          <t>Border Issues of Texas</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Contact: Shannon PensaEmail: brownsvillepreservationsociety@gmail.comPhone: 1-512-423-9442Address: 647 E. St. Charles StCity: Brownsville</t>
+          <t>Boy Scouts of America, Rio Grande Council</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Contact: Veronica RosenbaumEmail: brownsvillewellnesscoalition@gmail.comPhone: 1-956-465-4178Address: One West UniversityCity: BROWNSVILLE</t>
+          <t>Boys &amp; Girls Club of Harlingen</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Contact: Julian garciaEmail: julian.garcia@bt.churchPhone: 1-956-686-5296Address: 2001 Trenton RdCity: Mcallen</t>
+          <t>Boys &amp; Girls Club of McAllen</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Contact: Jorge RodriguezEmail: jrodriguez@buckner.orgPhone: 1-956-583-2041Address: 3780 N. Bentsen Palm DriveCity: Mission</t>
+          <t>Boys &amp; Girls Club of Mission</t>
         </is>
       </c>
     </row>
@@ -804,7 +804,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Contact: Patricia MartinezEmail: info@campuniversity.orgPhone: 1-956-560-1912Address: info@campuniversity.orgCity: McAllen</t>
+          <t>Boys &amp; Girls Club of Pharr</t>
         </is>
       </c>
     </row>
@@ -814,7 +814,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Contact: Guadalupe CastroEmail: guadalupe.castro@agnet.tamu.eduPhone: 1-956-361-8236Address: 1390 W. Expressway 83City: Brownsville</t>
+          <t>Boys &amp; Girls Club of Weslaco, Inc.</t>
         </is>
       </c>
     </row>
@@ -824,7 +824,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Contact: Anna De La CruzEmail: executivedirector@cccadvocacycenter.orgPhone: 1-956-361-3313Address: 1390 W. Expressway 83City: San Benito</t>
+          <t>Boys &amp; Girls Clubs of Edinburg RGV</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Contact: Valerie ArizmendiEmail: vrcariz@aol.comPhone: 1-956-245-7336Address: 500 E Ocean BlvdCity: Los Fresnos</t>
+          <t>Boys &amp; Girls Clubs of Los Fresnos</t>
         </is>
       </c>
     </row>
@@ -844,7 +844,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Contact: RoseEmail: rgomez@co.cameron.tx.usPhone: 1-956-399-3075Address: P.O Box 1690 San Benito.TX,78586City: San Benito</t>
+          <t>Bright Heart Project – Houston</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Contact: Elizabeth MartinezEmail: elizabeth217@me.comPhone: 1-956-821-8662Address: 2821 W. Canton Rd.City: Edinburg</t>
+          <t>Brownsville Community Foundation</t>
         </is>
       </c>
     </row>
@@ -864,7 +864,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Contact: Stephanie WilsonEmail: swilson@ckrgv.orgPhone: 1-956-433-5041Address: P.O. Box 13621City: Port Isabel</t>
+          <t>Brownsville Community Health Center</t>
         </is>
       </c>
     </row>
@@ -874,7 +874,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Contact: LettyEmail: Lguzman@wellmed.netPhone: 1-956-630-6667Address: 1301 E. Fern, McAllen, TX 78501City: Mcallen</t>
+          <t>Brownsville Historical Association</t>
         </is>
       </c>
     </row>
@@ -884,7 +884,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Contact: Hilda Ledezma/ Alejandro CruzEmail: carlottaculturalcenter@gmail.comPhone: 1-956-280-6522Address: 1452 E. MadisonCity: Brownsville</t>
+          <t>Brownsville Literacy Center</t>
         </is>
       </c>
     </row>
@@ -894,7 +894,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Contact: Maria or CeliaEmail: casamamimx@gmail.comPhone: 1-956-432-7202 (Maria); 1-956-793-6073 (Celia)Address: 2000 S. McColl Suite B #130, Mcallen TexasCity: McAllen</t>
+          <t>Brownsville Museum of Fine Art</t>
         </is>
       </c>
     </row>
@@ -904,7 +904,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Contact: Jose MedranoEmail: jmedrano@casaofcw.orgPhone: 1-956-546-6545Address: 1740 Boca Chica Blvd. #300City: Brownsville</t>
+          <t>Brownsville Preservation Society</t>
         </is>
       </c>
     </row>
@@ -914,7 +914,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Contact: Bianca LopezEmail: blopez@casaofhidalgo.comPhone: 1-956-381-0346Address: 1001 S 10th AveCity: Edinburg</t>
+          <t>Brownsville Wellness Coalition</t>
         </is>
       </c>
     </row>
@@ -924,7 +924,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Contact: Cesar MataEmail: volunteercoordinator@cdob.orgPhone: 1-956-897-3949Address: 1721 Beaumont Ave, McAllen, TX 78501City: McAllen</t>
+          <t>BT.Church McAllen</t>
         </is>
       </c>
     </row>
@@ -934,7 +934,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Contact: Yesenia GuzmanEmail: ytorre@cdob.orgPhone: 1-956-702-4088Address: 700 N. Virgen de San Juan Blvd.City: San Juan</t>
+          <t>Buckner Missions and Humanitarian Aid</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Contact: Dr. Laryssa MykytaEmail: laryssa.mykyta@utrgv.eduPhone: 1-956-665-3318Address: University of Texas Rio Grande ValleyCity: Edinburg</t>
+          <t>C.A.M.P. University</t>
         </is>
       </c>
     </row>
@@ -954,7 +954,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Contact: SantiagoEmail: sbaldazo@ChildFund.orgPhone: 1-956-681-3800Address: 1418 Beech Ave. McAllen, TX 78501City: McAllen</t>
+          <t>Cameron County 4-H</t>
         </is>
       </c>
     </row>
@@ -964,7 +964,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Contact: Gloria HernandezEmail: gloria.hernandez@cachidalgo.orgPhone: 1-956-287-9754Address: 525 W. Wisconsin Rd.City: Edinburg</t>
+          <t>Cameron County Children’s Advocacy Centers Inc.</t>
         </is>
       </c>
     </row>
@@ -974,7 +974,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Contact: Jesus SanchezEmail: jesus.sanchez@cachidalgo.orgPhone: 1-956-287-9754Address: 525 W. Wisconsin Rd.City: Edinburg</t>
+          <t>Cameron County Fair and Livestock Show</t>
         </is>
       </c>
     </row>
@@ -984,7 +984,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Contact: Randy BakerEmail: rbaker@cbs-rgv.orgPhone: 956-368-4065Address: 2302 S. 77 Sunshine StripCity: Harlingen</t>
+          <t>Cameron County Juvenile Probation</t>
         </is>
       </c>
     </row>
@@ -994,7 +994,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Contact: Felipe Peña IIIEmail: felipe@cmofbrownsville.comPhone: 1-956-547-6883Address: 501 Ringgold Street #5 Dean Porter ParkCity: Brownsville</t>
+          <t>Canterbury Elementary Parent Teacher Organization</t>
         </is>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Contact: Suzanne HerzingEmail: contact@cinderella-pet-rescue.orgPhone: 1-956-391-4399Phone: 1-956-638-9050Address: 307 W Orange Grove RdCity: Mission</t>
+          <t>Capable Kids Foundation</t>
         </is>
       </c>
     </row>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Contact: Terri LievanosEmail: rgsccvc@gmail.comPhone: 1-956-364-8255Address: 1401 Rangerville RdCity: Harlingen</t>
+          <t>Caregiver SOS by WellMed</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Contact: Samm MercadoEmail: samm.mercado@alton-tx.govPhone: 1-956-432-0790Address: 349 W. Dawes AveCity: Alton</t>
+          <t>Carlotta K. Petrina Cultural Center</t>
         </is>
       </c>
     </row>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Contact: Enrique Casas IIEmail: ecasas@cityofrgc.comPhone: 1-956-487-0672Address: 5332 E. Highway 83City: Rio Grande City</t>
+          <t>Casa Hogar MAMi in U.S.A</t>
         </is>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Contact: Stephanie BilodeauEmail: stephanie@cbbep.orgPhone: 1-802-309-5171Address: 615 N Upper BroadwayCity: Corpus Christi</t>
+          <t>CASA of Cameron &amp; Willacy Counties</t>
         </is>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Contact: DeYoe HudsonEmail: hudson.deyoe@utrgv.eduPhone: 1-956-761-2644Address: 100 Marine Lab Dr.,South Padre Island,TX,78597City: South Padre Island</t>
+          <t>CASA of Hidalgo County</t>
         </is>
       </c>
     </row>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Contact: JamesEmail: james.stockton01@utrgv.eduPhone: 1-956-802-5040</t>
+          <t>Catholic Charities Humanitarian Respite Center</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Contact: Irene WazgowskaEmail: Irene@codergv.orgPhone: 1-956-410-2633Address: 601 N Main StreetCity: McAllen</t>
+          <t>Catholic Charities of the Rio Grande Valley</t>
         </is>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Contact: EnriquetaEmail: kcaballero@sos.texas.govPhone: 1-956-969-9075Address: 255 S. Kansas Ave.City: Weslaco</t>
+          <t>Center for Survey Research &amp; Policy Analysis</t>
         </is>
       </c>
     </row>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Contact: BlancaEmail: colonias_unidas@yahoo.comPhone: 1-956-487-0964Address: 1 Las LomasCity: Rio Grande City</t>
+          <t>ChildFund International U.S. Program</t>
         </is>
       </c>
     </row>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Contact: Veronica WhitacreEmail: comforthouse617@yahoo.comPhone: 1-956-687-7367Address: 617 Dallas AvenueCity: McAllen</t>
+          <t>Children’s Advocacy Center of Hidalgo County, Inc./Estrella’s House</t>
         </is>
       </c>
     </row>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Contact: Jennifer BossoudahoEmail: evaperez@ciscameroncounty.orgPhone: 1-956-554-7954Address: 700 E. Levee St. Ste. 204City: Brownsville</t>
+          <t>Children’s Advocacy Center of Hidalgo County, Inc.</t>
         </is>
       </c>
     </row>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Contact: DavidEmail: cishidalgo@hotmail.comPhone: 1-956-630-0016Address: 3700 N 10th St, McAllen, TX 78501City: McAllen</t>
+          <t>Children’s Bereavement Center – RGV</t>
         </is>
       </c>
     </row>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Contact: Mark PearsonEmail: mark.pearson@communitiesu.orgPhone: 1-512-284-3000Address: 501 W Croslin StCity: Austin</t>
+          <t>Children’s Museum of Brownsville</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Contact: Sergio SalazarEmail: sergio.salazar@communitiesu.orgPhone: 1-956-689-1860Address: 700 FM 3168 STE 8 OFC 133City: Raymondville</t>
+          <t>Cinderella Pet Rescue</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Contact: Mary CantuEmail: mcantu@ccrgv.orgPhone: 1-956-532-7150Address: P.O. Box 182City: Weslaco</t>
+          <t>Citizens Volunteer Council for Rio Grande State Center</t>
         </is>
       </c>
     </row>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Contact: Abigail  TorreEmail: ccrgv@ccrgv.orgEmail: atorre@ccrgv.orgPhone: 1-956-447-4636Address: P.O. Box 182City: Weslaco</t>
+          <t>City of Alton Recreation Center</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Contact: Lupita VasquezEmail: lvasquez@ccrgv.orgPhone: 1-877-541-7905Address: P.O. Box 182City: Weslaco</t>
+          <t>City of Rio Grande City, Boys &amp; Girls Youth Club</t>
         </is>
       </c>
     </row>
@@ -1184,11 +1184,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Contact: Marcela Saenz 
-Email: msaenz@cdcb.org
-Phone: 1-956-541-4955
-Address: 901 E. Levee Street Brownsville, Tx. 78520
-City: Brownsville</t>
+          <t>Coastal Bend Bays &amp; Estuaries Program – Coastal Bird Program</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1194,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Contact: Thelma VasquezEmail: tvasquez@csa-hidalgo.usPhone: 1-956-383-6250Address: 2524 N. Closner BlvdCity: Edinburg</t>
+          <t>Coastal Studies Lab</t>
         </is>
       </c>
     </row>
@@ -1208,7 +1204,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Contact: Joel GonzalezEmail: Joelagonzalez@missionha.orgPhone: 1-956-585-9756Address: 1300 E. 8th St. Mission, TX 78572City: Mission</t>
+          <t>COBE Deans Office</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1214,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Contact: Joyce WeatherlyEmail: info@colmhealth.orgPhone: 1-956-970-9327Address: 2618 Louann LaneCity: Harlingen</t>
+          <t>Code RGV</t>
         </is>
       </c>
     </row>
@@ -1228,7 +1224,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Contact: Leonel VelaEmail: leonel.vela@hhsc.state.tx.us, leonel.vela@dshs.texas.govPhone: 1-956-971-1288Address: Office of Border Affairs, 4501 W Bus Hwy 83 McAllen, TX 78501City: McAllen</t>
+          <t>Colonia Initiatives Program</t>
         </is>
       </c>
     </row>
@@ -1238,7 +1234,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Contact: AurelioEmail: escasleal72@gmail.comPhone: 1-956-249-0382Address: 1308 Lark AveCity: McAllen</t>
+          <t>Colonias Unidas</t>
         </is>
       </c>
     </row>
@@ -1248,7 +1244,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Contact: MarioEmail: Donnahistoricalmuseum@yahoo.comPhone: 1-956-464-9989Address: 129 S 8th St, Donna, TX 78537City: Donna</t>
+          <t>Comfort House Services, Inc.</t>
         </is>
       </c>
     </row>
@@ -1258,7 +1254,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Contact: Martin EkoumouEmail: mekoumou@dlhope.orgPhone: 1-956-739-9702Address: P.O Box 3307City: McAllen</t>
+          <t>Communities in Schools of Cameron County</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1264,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Contact: SarahEmail: sarahrmchavez@gmail.comPhone: sarahrmchavez@gmail.comAddress: 505 W. Cano StreetCity: Edinburg</t>
+          <t>Communities in Schools of Hidalgo County</t>
         </is>
       </c>
     </row>
@@ -1278,7 +1274,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Contact: Rebekah Harrison; Patricia RosenlundEmail: rharrison@easterseals-rgv.org; prosenlund@easterseals-rgv.orgPhone: 1-956-631-9171 (Rebekah);  1-956-631-9171 ext 103 (Patricia) Address: 1217 W Houston AveCity: McAllen</t>
+          <t>Communities Unlimitied, Inc.</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1284,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Contact: SteveEmail: jgaytan@regencyhealthcare.comPhone: 1-956-541-0917Address: 1001 Central Blvd, Brownsville, TX 78520City: Brownsville</t>
+          <t>Community Council RGV (211 Texas Presentation or Health Fairs)</t>
         </is>
       </c>
     </row>
@@ -1298,7 +1294,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Contact: Dr. RosalindaEmail: rosalinda@ecolorsineducation.orgPhone: 1-281-202-9392Address: 8240 No. Mopac Expressway, Suite 130 P.O. Box 2031City: Austin</t>
+          <t xml:space="preserve">cdcb | come dream. come build. </t>
         </is>
       </c>
     </row>
@@ -1308,7 +1304,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Contact: Magdiel CastleEmail: magdiel@edinburglibrary.usPhone: 1-956-383-6246Address: 1906 S. Closner BlvdCity: Edinburg</t>
+          <t>Community Service Agency, County of Hidalgo</t>
         </is>
       </c>
     </row>
@@ -1318,7 +1314,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Contact: GylmaEmail: edinburgchildcare@hotmail.comPhone: 1-956-383-6789Address: 1332 W. University Dr. Edinburg, TX 78539City: Edinburg</t>
+          <t>Coto De Casa Inc.</t>
         </is>
       </c>
     </row>
@@ -1328,7 +1324,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Contact: Zeeshan NoorEmail: znoor@edinburgha.orgPhone: 1-956-383-3839Address: 910 S. Sugar RdCity: Edinburg</t>
+          <t>Culture of Life Ministries</t>
         </is>
       </c>
     </row>
@@ -1338,7 +1334,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Contact: Monica BarreraEmail: mbarrera@cityofedinburg.comPhone: 1-956-381-9922Address: 714 S. Raul Longoria Rd.City: Edinburg</t>
+          <t>Department of Health and Human Services DSHS/HHSC</t>
         </is>
       </c>
     </row>
@@ -1348,7 +1344,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Contact: LolitaEmail: Lolitapagarani@aol.comPhone: 1-956-789-4549Address: 1912 Martin AvenueCity: McAllen</t>
+          <t>Different Not Less dba AWARE-RGV</t>
         </is>
       </c>
     </row>
@@ -1358,7 +1354,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Contact: MichaelEmail: seifertjamesmichael@gmail.comEmail: november61954@gmail.comPhone: 1-956-459-6827Address: 1314 W St. Charles Brownsville 78520City: Brownsville</t>
+          <t>Donna Hooks Flethcer Museum Inc.</t>
         </is>
       </c>
     </row>
@@ -1368,7 +1364,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Contact: JaineEmail: Jchapa@cityofedinburg.comPhone: 1-956-292-2133 ext.1119Address: 3102 S Business Highway 281, Edinburg, TX 78539City: Edinburg</t>
+          <t>Don’t Lose Hope (DLH)</t>
         </is>
       </c>
     </row>
@@ -1378,7 +1374,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Contact: Monica BarreraEmail: mbarrera@cityofedinburg.comPhone: 1-956-381-9922Address: 714 S. Raul Longoria Rd.City: Edinburg</t>
+          <t>Dream Home/RGV Pride Home INC</t>
         </is>
       </c>
     </row>
@@ -1388,7 +1384,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Contact: LolitaEmail: Lolitapagarani@aol.comPhone: 1-956-789-4549Address: 1912 Martin AvenueCity: McAllen</t>
+          <t>Easter Seals Rio Grande Valley</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1394,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Contact: MichaelEmail: seifertjamesmichael@gmail.comEmail: november61954@gmail.comPhone: 1-956-459-6827Address: 1314 W St. Charles Brownsville 78520City: Brownsville</t>
+          <t>Ebony Lake Health Care Center</t>
         </is>
       </c>
     </row>
@@ -1408,7 +1404,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Contact: UribeEmail: joe.uribe@tpwd.texas.govPhone: 1-956-565-3919Address: 154-A Lakeview DrCity: Weslaco TX</t>
+          <t>E-Colors in Education</t>
         </is>
       </c>
     </row>
@@ -1418,7 +1414,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Contact: RosalvaEmail: Ropuente85@gmail.comPhone: 1-956-579-7234Address: 1105 S SugarCity: Edinburg</t>
+          <t>Edinburg Arts, Dustin Michael Sekula Memorial Library</t>
         </is>
       </c>
     </row>
@@ -1428,7 +1424,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Contact: YeseniaEmail: yesenia.ramirez1.ctr@mail.milPhone: 1-956-969-1912Address: 1100 Vo-Tech DrCity: Weslaco</t>
+          <t>Edinburg Child Care Inc.</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1434,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Contact: Adrianna HernandezEmail: ahernandezfcc@sbcglobal.netPhone: 1-956-423-9305Address: 616 W. TaylorCity: Harlingen</t>
+          <t>Edinburg Housing Authority</t>
         </is>
       </c>
     </row>
@@ -1448,7 +1444,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Contact: HannahEmail: fpcweslacotx@gmail.comPhone: 1-956-969-1535City:Weslaco</t>
+          <t>Edinburg Scenic Wetlands &amp; World Birding Center</t>
         </is>
       </c>
     </row>
@@ -1458,7 +1454,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Contact: RalphEmail: notpit73@gmail.comPhone: 1-956-561-9268Address: 302 Kings HwyCity: Brownsville</t>
+          <t>EmPOWER R.G.V.</t>
         </is>
       </c>
     </row>
@@ -1468,7 +1464,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Contact: JillianEmail: jillian.freshink@gmail.com</t>
+          <t>Equal Voice Network</t>
         </is>
       </c>
     </row>
@@ -1478,7 +1474,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Contact: AnnEmail: gcharlton@rgv.rr.comPhone: 1-956-968-2419Address: 1023 Bella Vista Weslaco, TX 78596City: Weslaco</t>
+          <t>Edinburg Recycling Center</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1484,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Contact: Evonne LopezEmail: communityed@fowinc.comPhone: 1-956-544-7412Address: 95 E. Price Rd. Suite CCity: Brownsville</t>
+          <t>Estero Llano Grande State Park</t>
         </is>
       </c>
     </row>
@@ -1498,7 +1494,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Contact: Chris WarrenEmail: fronteraaudubon@gmail.comPhone: 1-956-968-3275Address: 1101 S. Texas BlvdCity: Weslaco</t>
+          <t>Faith Sparked Passion</t>
         </is>
       </c>
     </row>
@@ -1508,7 +1504,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Contact: HectorEmail: fightwagetheft@gmail.comPhone: 1-956-283-5650Address: Rio Grande ValleyCity: RGV</t>
+          <t>Family Assistance Center</t>
         </is>
       </c>
     </row>
@@ -1518,7 +1514,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Contact: Amencio AlmanzaEmail: aalmanza9@gmail.comPhone: 1-956-563-0877Address: 4114 E. Lopez Dr.City: Edinburg</t>
+          <t>Family Crisis Center</t>
         </is>
       </c>
     </row>
@@ -1528,7 +1524,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Contact: Adriana EstradaEmail: adriana.estrada@gencure.orgPhone: 1-210-857-5990Address: 6211 IH 10 WestCity: San Antonio</t>
+          <t>First Presbyterian Church</t>
         </is>
       </c>
     </row>
@@ -1538,7 +1534,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Contact: JeanEmail: jean.pena@gentiva.comPhone: 1-956-423-1101Address: 410 A Ed Carey DriveCity: Harlingen</t>
+          <t>Francisco S. Tipton Law Firm</t>
         </is>
       </c>
     </row>
@@ -1548,7 +1544,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Contact: Janie PerezEmail: jperez@gsgst.orgPhone: 1-956-425-2388Address: 202 E. MadisonCity: Harlingen</t>
+          <t>Freshink</t>
         </is>
       </c>
     </row>
@@ -1558,7 +1554,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Contact: Terry BlevinsEmail: tblevins@gsgst.orgPhone: 1-956-668-0299Address: 5317 N. McColl RdCity: McAllen</t>
+          <t>Friends of the Weslaco Library</t>
         </is>
       </c>
     </row>
@@ -1568,7 +1564,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Contact: Melissa MuzquizEmail: melissa.muzquiz@girlsontherun.orgPhone: 1-956-459-0717Address: P.O. Box 5901City: Brownsville</t>
+          <t>Friendship of Women Inc.</t>
         </is>
       </c>
     </row>
@@ -1578,7 +1574,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Contact: Alicia MolinaEmail: educ@gpz.orgPhone: 1-956-546-7187Address: 500 Ringgold StCity: Brownsville</t>
+          <t>Frontera Audubon</t>
         </is>
       </c>
     </row>
@@ -1588,7 +1584,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Contact: Judith Rodriguez; Belinda BradfordEmail: judith.rodriguez02@utrgv.edu; BBradford@goodneighborsettlement.orgPhone: 1-956-542-2368Address: 1254 E. TylerCity: Brownsville</t>
+          <t>Fuerza del Valle Workers’ Center</t>
         </is>
       </c>
     </row>
@@ -1598,7 +1594,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Contact: Lukas SehlkeEmail: volunteer.coordinator@goodsamtx.orgPhone: 1-210-434-5531Address: 104 W Elizabeth StCity: Brownsville</t>
+          <t>Game Changers McTX</t>
         </is>
       </c>
     </row>
@@ -1608,7 +1604,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Contact: Alicia StewartEmail: volunteer.coordinator@goodsamtx.orgAddress: 317 W. GoreCity: Pharr</t>
+          <t>GenCure Marrow Donor Program – Be The Match</t>
         </is>
       </c>
     </row>
@@ -1618,7 +1614,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Contact: Sara SaenzEmail: ssaenz@goodwillsouthtexas.comPhone: 1-956-383-0023Address: 3502 S. I-69</t>
+          <t>Gentiva Hospice Foundation</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1624,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Contact: Aldo ChapaEmail: graciahospicecare@yahoo.comPhone: 1-956-661-1177Address: 717 E. Esperanza Ave.City: Mcallen</t>
+          <t>Girl Scouts of Greater South Texas (Harlingen)</t>
         </is>
       </c>
     </row>
@@ -1638,7 +1634,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Contact: Alexa AragonEmail: aaragon@guadalupeprep.orgPhone: 1-956-504-5568Address: 1214 Lincoln St.City: Brownsville</t>
+          <t>Girl Scouts of Greater South Texas (McAllen)</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1644,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Contact: Janine Marie CampbellEmail: haef@hcisd.orgPhone: 1-956-499-3285Address: P.O. BOX 521328City: Harlingen</t>
+          <t>Girls on the Run RGV</t>
         </is>
       </c>
     </row>
@@ -1658,7 +1654,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Contact: Don RinearsonEmail: kathyrinearson@gmail.comPhone: 1-260-466-1607Address: 115 Jackson StreetCity: Harlingen</t>
+          <t>Gladys Porter Zoo</t>
         </is>
       </c>
     </row>
@@ -1668,7 +1664,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Contact: Rose TimmerEmail: hcb@healthybrownsville.orgPhone: 1-956-543-5404Address: One West University BlvdCity: Brownsville</t>
+          <t>Good Neighbor Settlement House, Inc.</t>
         </is>
       </c>
     </row>
@@ -1678,7 +1674,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Contact: DanikaEmail: danikajean03@outlook.comPhone: 1-956-369-7846Address: 100 E Cano St.City: Edinburg</t>
+          <t>Good Samaritan Community Services, Cameron County</t>
         </is>
       </c>
     </row>
@@ -1688,7 +1684,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Contact: Rose TimmerEmail: hcb@healthybrownsville.orgPhone: 1-956-543-5404Address: One West University BlvdCity: Brownsville</t>
+          <t>Good Samaritan Community Services, Pharr</t>
         </is>
       </c>
     </row>
@@ -1698,7 +1694,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Contact: Cynthia CatchingsEmail: cyntheph@yahoo.comPhone: 1-956-438-2805Address: 4800 N 10th Ste. DCity: McAllen</t>
+          <t>Goodwill Industries of South Texas</t>
         </is>
       </c>
     </row>
@@ -1708,7 +1704,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Contact: Eliza GomezEmail: eliza.gomez@hchd.orgPhone: 1-956-318-2426City: Edinburg</t>
+          <t>Gracia Hospice LLC.</t>
         </is>
       </c>
     </row>
@@ -1718,7 +1714,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Contact: NancyEmail: nancy.trevino@hchd.orgPhone: 1-956-383-6221 ext. 7337Address: 1304 South 25th AveCity: Edinburg</t>
+          <t>Guadalupe Regional Middle School</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1724,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Contact: Jaime GaonaEmail: jgaona@cityofhidalgo.netPhone: 1-956-843-9762Address: 122 N. 2nd St.City: Hidalgo</t>
+          <t>Harlingen Area Educational Foundation</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1734,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Contact: Sandra de la Cruz-YarrisonEmail: holyfamilybirthcenter@gmail.comPhone: 1-956-969-2538Address: 5819 North FM 88City:Weslaco</t>
+          <t>Harlingen Art Forum</t>
         </is>
       </c>
     </row>
@@ -1748,7 +1744,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Contact: Melissa LandinEmail: mellyanna@yahoo.comPhone: 1-956-455-7044Address: 643 Rey SalomonCity: Brownsville</t>
+          <t>Healthy Communities of Brownsville, Inc</t>
         </is>
       </c>
     </row>
@@ -1758,7 +1754,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Contact: Nancy or RebeccaEmail: ngsaenz.hfhc@gmail.com; rramirez.hfhc@gmail.comPhone: 1-956-994-3319 Address: 2332 Jordan Rd W, McAllen, TX 78503City: McAllen</t>
+          <t>Hidalgo County D.A. Office</t>
         </is>
       </c>
     </row>
@@ -1768,7 +1764,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Contact: Diana PadillaEmail: hopeforsfs@yahoo.comPhone: 1-956-412-4916Address: 19833 Morris RoadCity: Harlingen</t>
+          <t>Hidalgo County Family Violence Task Force</t>
         </is>
       </c>
     </row>
@@ -1778,7 +1774,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Contact: JoePhone: 1-956-784-2016Address: 2011 Verdin Ave Mcallen, TX 78504City: McAllen</t>
+          <t>Hidalgo County Health &amp; Human Services Department</t>
         </is>
       </c>
     </row>
@@ -1788,7 +1784,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Contact: Vicki SaenzEmail: ifnargv@gmail.comPhone: 1-956-541-9250Address: 1225 Boca Chica Blvd.City: Brownsville</t>
+          <t>Hidalgo County Health and Human Services</t>
         </is>
       </c>
     </row>
@@ -1798,7 +1794,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Contact: GloriaEmail: visitorcenter@mma-tx.orgPhone: 1-956-421-9201Address: 320 Iwo Jima Blvd. Harlingen, TX 78550City: Harlingen</t>
+          <t>Hidalgo Youth Center</t>
         </is>
       </c>
     </row>
@@ -1808,7 +1804,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Contact: X. David GonzalezEmail: dagonzalez@justenergy.comPhone: 1-956-639-0588Address: 609 Vine AveCity: McAllen</t>
+          <t>Holy Family Services</t>
         </is>
       </c>
     </row>
@@ -1818,7 +1814,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Contact: Eli De LeonEmail: kbb.texas@gmail.comPhone: 1-956-459-1631Address: 6035 Jaime J. ZapataCity: Brownsville</t>
+          <t>Hooked for Life Kids Gone Fish’n</t>
         </is>
       </c>
     </row>
@@ -1828,7 +1824,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Contact: Chris LashEmail: kmb@mcallen.netPhone: 1-956-681-4562Address: P O Box 220City: McAllen</t>
+          <t>Hope Family Health Center</t>
         </is>
       </c>
     </row>
@@ -1838,7 +1834,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Contact: Becky GraciaEmail: kmb@cityofmercedes.comPhone: 1-956-565-3114Address: 400 S. Ohio Ave.City: Mercedes</t>
+          <t>HOPE for Small Farms Sustainability</t>
         </is>
       </c>
     </row>
@@ -1848,7 +1844,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Contact: Lynne PareEmail: keepsanbenitobeautiful@yahoo.comPhone: 1-956-241-0915Address: PO Box 1513City: San Benito</t>
+          <t>Hope In Joy</t>
         </is>
       </c>
     </row>
@@ -1858,7 +1854,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Contact: Mel or YvonneEmail: mel@knappccf.com; bonnie@knappccf.comPhone: 1-956-854-4534Address: P.O. Box 1790City: Weslaco</t>
+          <t>Infant and Family Nutrition Agency</t>
         </is>
       </c>
     </row>
@@ -1868,7 +1864,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Contact: Imelda AmbrizEmail: iambriz@primehealthcare.comPhone: 1-956-973-5144Address: 1401 E. 8th StreetCity: Weslaco</t>
+          <t>Iwo Jima Museum</t>
         </is>
       </c>
     </row>
@@ -1878,7 +1874,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Contact: JaimeEmail: jsandoval@cityoflaferia.comPhone: 1-956-797-2261Address: 115 E. Commercial Ave.City:La Feria</t>
+          <t>Just Energy</t>
         </is>
       </c>
     </row>
@@ -1888,7 +1884,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Contact: Sister ZitaEmail: zitacdp@gmail.comPhone: 1-956-399-3826Address: 1610 Marydale RdCity: San Benito</t>
+          <t>Keep Brownsville Beautiful</t>
         </is>
       </c>
     </row>
@@ -1898,7 +1894,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Contact: Tania ChavezEmail: taniac@lupenet.orgPhone: 1-956-648-0786Address: 1601 E. Business Highway 83, PO Box 188City: San Juan</t>
+          <t>Keep McAllen Beautiful, Inc.</t>
         </is>
       </c>
     </row>
@@ -1908,7 +1904,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Contact: Marion MasonEmail: Marion_Mason@fws.govPhone: 1-956-748-3607Address: 22688 Buena Vista RdCity: Los Fresnos</t>
+          <t>Keep Mercedes Beautiful</t>
         </is>
       </c>
     </row>
@@ -1918,7 +1914,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Contact: BoydEmail: boyd_blihovde@fws.govPhone: 1-956-748-3607 x104Address: 22817 Ocelot RoadCity: Los Fresnos</t>
+          <t>Keep San Benito Beautiful</t>
         </is>
       </c>
     </row>
@@ -1928,7 +1924,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Contact: Marcela HancockEmail: mhancock@lagunamadrekids.orgPhone: 1-956-943-6310Address: 190 Port RoadCity: Port Isabel</t>
+          <t>Knapp Community Care Foundation</t>
         </is>
       </c>
     </row>
@@ -1938,7 +1934,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Contact: Pastor BillEmail: office@tbmcallen.comPhone: 1-956-686-4679Address: 2001 Freddy Gonzalez Dr, McAllen, TX 78504City: McAllen</t>
+          <t>Knapp Medical Center</t>
         </is>
       </c>
     </row>
@@ -1948,7 +1944,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Contact: OrlandoEmail: orlando.salinas@llanogrande.orgPhone: 1-956-262-4474Address: 1 Yellow Jacket Dr. Ste 1 A, Edcouch, TX 78538City: Edcouch</t>
+          <t>La Feria Community Resource Center</t>
         </is>
       </c>
     </row>
@@ -1958,7 +1954,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Contact: Bill ReaganEmail: office@lfrgv.orgPhone: 1-956-423-1014Address: 514 South E St.City: Harlingen</t>
+          <t>La Posada Providencia Shelter</t>
         </is>
       </c>
     </row>
@@ -1968,7 +1964,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Contact: JuanaEmail: juana.escareno@lrgvahec.comPhone: 1-956-296-1459Address: 108 N Jackson Rd, Suite 108City: Edinburg</t>
+          <t>La Unión del Pueblo Entero (LUPE)</t>
         </is>
       </c>
     </row>
@@ -1978,7 +1974,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Contact: ArmandoEmail: armando.lopez@lrgvahec.comPhone: 1-956-357-7270Address: 108 N Jackson Rd, Suite 108City: Edinburg</t>
+          <t>Laguna Atascosa National Wildlife Refuge</t>
         </is>
       </c>
     </row>
@@ -1988,7 +1984,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Contact: Marcie OviedoEmail: rongarza@lrgvdc.orgPhone: 1-956-682-3481Address: 301 W. RailroadCity: Weslaco</t>
+          <t>Laguna Atascosa NWR</t>
         </is>
       </c>
     </row>
@@ -1998,7 +1994,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Contact: Juanita SaenzEmail: jsaenz@lrgvdc.orgPhone: 1-956-682-3481Address: 301 W. Railroad St.City: Weslaco</t>
+          <t>Laguna Madre Youth Center</t>
         </is>
       </c>
     </row>
@@ -2008,7 +2004,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Contact: Miriam SuarezEmail: mainstreet@cob.usPhone: 1-956-548-6156Address: 1034 E. Levee StreetCity: Brownsville</t>
+          <t>LDS Church</t>
         </is>
       </c>
     </row>
@@ -2018,7 +2014,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Contact: Ava SandlinEmail: asandlin@rgv.wish.orgPhone: 1-956-686-9474Address: 1801 S. 2nd Street, Suite 405City: McAllen</t>
+          <t>Llano Grande Center for Research and Development</t>
         </is>
       </c>
     </row>
@@ -2028,7 +2024,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Contact: KarinaEmail: karinamichellecerda@tamu.eduPhone: 1-956-668-0060Address: 2402 Cornerstone BlvdCity: Edinburg</t>
+          <t>Loaves &amp; Fishes of the RGV, Inc.</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2034,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Contact: Jose Luis Adame Jr.Email: jladame@mcallencareersinstitute.comPhone: 1-956-618-5800Address: 304 S Col. Rowe Blvd.City: McAllen</t>
+          <t>Lower Rio Grande Valley Area Health Education Center (LRGV AHEC)</t>
         </is>
       </c>
     </row>
@@ -2048,7 +2044,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Contact: Kristina Y. Garza or Cristina MonroyEmail: mccvolunteers@mcallen.netPhone: 1-956-681-3800Address: 701 Convention Center Blvd.City: McAllen</t>
+          <t>Lower Rio Grande Valley Development Council</t>
         </is>
       </c>
     </row>
@@ -2058,7 +2054,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Contact: Piedad MartinezEmail: pmartinez@mcallen.netPhone: 1-956-605-0630Address: 1601 N. Bicentennial BlvdCity: McAllen</t>
+          <t>LRGVDC Citizen Corps</t>
         </is>
       </c>
     </row>
@@ -2068,7 +2064,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Contact: Elva M. CerdaEmail: ecerda@mcallenheritagecenter.comPhone: 1-956-681-2861  Address: 301 S Main StCity: McAllen</t>
+          <t>Main Street Brownsville</t>
         </is>
       </c>
     </row>
@@ -2078,7 +2074,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Contact: Kristyna ManciasEmail: volunteerMHP@mcallen.netPhone: 1-956-681-3333Address: 2001 N. BicentennialCity: McAllen</t>
+          <t>Make-A-Wish Rio Grande Valley</t>
         </is>
       </c>
     </row>
@@ -2088,7 +2084,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Contact: Sandra SanchezEmail: ssanchez@themonitor.comPhone: 1-956-605-0470Address: Operating out of The MonitorCity: McAllen</t>
+          <t>Marquez Robotic Orthopedic Institute</t>
         </is>
       </c>
     </row>
@@ -2098,7 +2094,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Contact: Sarai GarciaEmail: sgarcia@mcallen.netPhone: 1-956-681-3333Address: 1000 S Ware RdCity: McAllen</t>
+          <t>McAllen Careers Institute</t>
         </is>
       </c>
     </row>
@@ -2108,7 +2104,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Contact: Tiffany KerstenEmail: tkersten@mcallen.netPhone: 1-956-681-3333Address: 4101 W Business 83City: McAllen</t>
+          <t>McAllen Convention Center</t>
         </is>
       </c>
     </row>
@@ -2118,7 +2114,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Contact: StevenEmail: skirpes@hiline.netPhone: 1-956-380-2930Address: PO BOX 4523City: Edinburg</t>
+          <t>McAllen Crime Stoppers</t>
         </is>
       </c>
     </row>
@@ -2128,7 +2124,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Contact: hanani vasquezEmail: hanani.vasquez@stisd.netPhone: 1-926-204-1737Address: 106500 North Expressway 77/83City: Olmito</t>
+          <t>McAllen Heritage Center</t>
         </is>
       </c>
     </row>
@@ -2138,7 +2134,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Contact: ChrisEmail: CYanas@mhm.orgPhone: 1-210-692-0234Address: 4507 Medical DriveCity: San Antonio</t>
+          <t>McAllen Holiday Parade</t>
         </is>
       </c>
     </row>
@@ -2148,7 +2144,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Contact: Dr. JohnEmail: jlowdermilk@mac.comPhone: 1-859-536-9857Address: 2212 River Drive, Edinburg TX, 78539City: Edinburg</t>
+          <t>McAllen Kids Marathon, City of McAllen</t>
         </is>
       </c>
     </row>
@@ -2158,7 +2154,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Contact: Maggie Dante, Ph.D, LMHCEmail: magaly.dante@mhpsalud.orgPhone: 1-956-904-5428Address: 3102 U.S. 83 Business GCity: Weslaco</t>
+          <t>McAllen Marathon, City of McAllen</t>
         </is>
       </c>
     </row>
@@ -2168,7 +2164,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Contact: Sarah MyersEmail: MilamMustangPTO@gmail.comPhone: 1-956-971-4333Address: 3800 N. Main St.City: McAllen</t>
+          <t>McAllen Nature Center</t>
         </is>
       </c>
     </row>
@@ -2178,7 +2174,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Contact: Dina RodriguezEmail: miraclekidsofsouthtexas@gmail.comPhone: 1-956-457-3941Address: PO Box 5281City: McAllen</t>
+          <t>McAllen Stamp Club</t>
         </is>
       </c>
     </row>
@@ -2188,7 +2184,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Contact: EricEmail: eeolivarez@gmail.comPhone: 1-956-240-1949Address: 910 E 2ND STCity: Mission</t>
+          <t>Medical Academy HOSA</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2194,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Contact: Christine CavazosEmail: ccavazos@moodyclinic.orgPhone: 1-956-542-8504Address: 1901 E. 22nd StCity: Brownsville</t>
+          <t>Methodist Healthcare Ministries</t>
         </is>
       </c>
     </row>
@@ -2208,7 +2204,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Contact: AnaEmail: south.tx@madd.orgEmail: ana.verley@madd.orgEmail: cynthia.sauceda@madd.orgPhone: 1-956-682-5928Address: 4751 South Jackson RoadCity: EdinburgAddress: 1763 Military HwyCity: Brownsville</t>
+          <t>Mexican Border Children Fund</t>
         </is>
       </c>
     </row>
@@ -2218,7 +2214,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Contact: Jerry MoralesEmail: jmorales@mosthistory.orgPhone: 1-956-383-6911Address: 200 N. Closner Blvd.City: Edinburg</t>
+          <t xml:space="preserve">MHP Salud </t>
         </is>
       </c>
     </row>
@@ -2228,7 +2224,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Contact: Max MunozEmail: max@nationalbutterflycenter.orgPhone: 1-956-583-5400Address: 3333 Butterfly Park Dr.City: Mission</t>
+          <t>Milam Elementary PTO</t>
         </is>
       </c>
     </row>
@@ -2238,7 +2234,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Contact: Ana VasquezEmail: nevaehskcc@gmail.comPhone: 1-956-221-2464Address: 4610 S. ClosnerCity: Edinburg</t>
+          <t>Miracle Kids of South Texas</t>
         </is>
       </c>
     </row>
@@ -2248,7 +2244,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Contact: MarcoEmail: marco_davis@newprofit.orgPhone: 1-202-930-5517Address: 200 Clarendon Street, 44th FloorCity: Boston</t>
+          <t>Mission Firemens Entrust</t>
         </is>
       </c>
     </row>
@@ -2258,7 +2254,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Contact: JennyEmail: newcombandassociates@gmail.comPhone: 1-956 665-7566Address: 1024 W. MapleCity: Mission</t>
+          <t>Moody Clinic</t>
         </is>
       </c>
     </row>
@@ -2268,7 +2264,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Contact: Rebecca LermaEmail: Rebecca.lerma@mcallenisd.netPhone: 1-956-429-1609Address: 2101 N Ware Rd.City: McAllen</t>
+          <t>Mothers Against Drunk Driving- South Texas</t>
         </is>
       </c>
     </row>
@@ -2278,7 +2274,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Contact: ClaudiaPhone: 1-956-763-2328Address: 2010 E. main Ave.City: Mission</t>
+          <t>Museum of South Texas History</t>
         </is>
       </c>
     </row>
@@ -2288,7 +2284,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Contact: GilbertEmail: k.valadez@nuevaluzfoundation.orgEmail: info@nuevaluzfoundation.orgPhone: 1-956-351-5653Address: 902 S Airport ste. 7City: Weslaco</t>
+          <t>National Butterfly Center</t>
         </is>
       </c>
     </row>
@@ -2298,7 +2294,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Contact: Jeanette AhleniusEmail: jahlenius596@gmail.comPhone: 1-956-212-0221Address: 1600 HarveyCity: McAllen</t>
+          <t>Nevaeh’s Kidz Conquering Cancer</t>
         </is>
       </c>
     </row>
@@ -2308,7 +2304,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Contact: InezEmail: cervantes.inez@gmail.comPhone: 1-616-514-8101</t>
+          <t>New Profit, Inc.</t>
         </is>
       </c>
     </row>
@@ -2318,7 +2314,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Contact: BonnieEmail: mrealty@prontonet.netPhone: 1-956-689-3600Address: 957 E. Hidalgo AvenueCity: Raymondville</t>
+          <t>Newcomb and Associates</t>
         </is>
       </c>
     </row>
@@ -2328,7 +2324,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Contact: Elizabeth or Anna MariaEmail: Liz@onestarfoundation.org; amfarias42@gmail.comPhone: 1-512-287-2062 (Liz); 1-571-2287041 (Anna Maria)Address: 9011 Mountain Ridge Drive Suite 100City: Austin</t>
+          <t>Nikki Rowe High School Interact Club</t>
         </is>
       </c>
     </row>
@@ -2338,7 +2334,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Contact: Arturo AscencionEmail: r2d23292@gmail.comPhone: 1-956-585-2623Address: 609 S ConwayCity: Mission</t>
+          <t>No Bullying in School</t>
         </is>
       </c>
     </row>
@@ -2348,7 +2344,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Contact: Victor MaldonadoEmail: victor@ozanamcenter.orgPhone: 1-956-831-6331Address: 656 N. Minnesota AveCity: Brownsville</t>
+          <t>Nueva Luz Foundation</t>
         </is>
       </c>
     </row>
@@ -2358,7 +2354,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Contact: Roger AstudilloEmail: rogelio.astudillo@co.hidalgo.tx.usPhone: 1-956-784-3505Address: 1429 S. Tower RdCity: Alamo</t>
+          <t>One Starfish Ministry</t>
         </is>
       </c>
     </row>
@@ -2368,7 +2364,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Contact: Debbie RockelmannEmail: deborah@pvaconline.comPhone: 1-956-686-1141Address: 2501 W. TrentonCity: Edinburg</t>
+          <t>One Way</t>
         </is>
       </c>
     </row>
@@ -2378,7 +2374,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Contact: Nadia OchoaEmail: nadia.pdap@gmail.comPhone: 1-956-687-7714Address: 115 N. 9th St.City: McAllen</t>
+          <t>OneStar Foundation</t>
         </is>
       </c>
     </row>
@@ -2388,7 +2384,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Contact: Araceli CasaresEmail: pctpharr@gmail.comPhone: 1-956-502-8145Address: 213 W. Newcombe AveCity: Pharr</t>
+          <t>OneStar Foundation – Austin</t>
         </is>
       </c>
     </row>
@@ -2398,7 +2394,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Contact: KarinaEmail: karina.lopez@pharr-tx.govPhone: 1-956-402-4332Address: 1215 S. Cage Blvd.City: Pharr</t>
+          <t>Our Lady of Guadalupe Catholic Church-Pantry</t>
         </is>
       </c>
     </row>
@@ -2408,7 +2404,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Contact: Somer PerezEmail: Somer.perez@pharrha.orgPhone: 1-956-787-1822Address: 104 W. Polk AveCity: Pharr</t>
+          <t>Ozanam Center</t>
         </is>
       </c>
     </row>
@@ -2418,7 +2414,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Phone: 1-956-943-2262Address: 421 Queen Isabella BlvdCity: Port Isabel</t>
+          <t>P2 Alamo Community Resource Center</t>
         </is>
       </c>
     </row>
@@ -2428,7 +2424,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Contact: Jessica HilarioEmail: jessica@prcrgv.comPhone: 1-956-519-9997Address: 216 E. Tom LandryCity: Mission</t>
+          <t>Palm Valley Animal Center</t>
         </is>
       </c>
     </row>
@@ -2438,7 +2434,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Contact: MarshaEmail: marshanelson@rgv.rr.comPhone: 1-956-802-9993Address: 2519 S. Inspiration Rd.City: Mission</t>
+          <t>Palmer Drug Abuse Program-McAllen</t>
         </is>
       </c>
     </row>
@@ -2448,7 +2444,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Contact: NoemiEmail: noemi.salas4@gmail.comPhone: 1-956-547-1017City: Brownsville</t>
+          <t>Pharr Community Theater &amp; Cultural Arts</t>
         </is>
       </c>
     </row>
@@ -2458,7 +2454,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Contact: Ann CassEmail: annwcass@aol.comPhone: 1-956-702-3307Address: 1212 U.S. 83 BusinessCity: San Juan</t>
+          <t>Pharr Economic Development Corporation II</t>
         </is>
       </c>
     </row>
@@ -2468,7 +2464,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Contact: Sr.Fatima SantiagoEmail: proyectodesarrollohumanotexas@gmail.comPhone: 1-956-580-9726Address: 17617 Sabal Palm DriveCity: Penitas</t>
+          <t>Pharr Housing Authority</t>
         </is>
       </c>
     </row>
@@ -2478,7 +2474,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Contact: Noemi SantanaEmail: Noemi.Santana@proyecto-jd.orgPhone: 1-956-542-2488Address: 2216 Eduardo AvenueCity: Brownsville</t>
+          <t>Port Isabel Chamber of Commerce</t>
         </is>
       </c>
     </row>
@@ -2488,7 +2484,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Contact: Jose Luis ZunigaEmail: JLZuniga@McAllen.netPhone: 1-956-681-3370Address: 600 Sunset DriveCity: McAllen</t>
+          <t>Pregnancy Resource Centers</t>
         </is>
       </c>
     </row>
@@ -2498,7 +2494,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Contact: GabrielEmail: jinglebells333@hotmail.comEmail: gabe.lozano@racksandtusks.orgPhone: 1-956-383-1077Address: PO Box 3305City: Edinburg</t>
+          <t>Project Insight (El Rocio Retreat)</t>
         </is>
       </c>
     </row>
@@ -2508,7 +2504,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Contact: Valerie AparicioEmail: v_aparicio2002@yahoo.comPhone: 1-956-689-1864Address: 700 FM 3168City: Raymondville</t>
+          <t>Project Space</t>
         </is>
       </c>
     </row>
@@ -2518,7 +2514,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Contact: Cesar GarciaEmail: rccc@recoverycentercc.orgPhone: 1-956-548-0028Address: 700 E. Levee Suite 101City: Brownsville</t>
+          <t>Proyecto Azteca</t>
         </is>
       </c>
     </row>
@@ -2528,7 +2524,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Contact: Denise AnayaEmail: danaya@esc1.netPhone: 1-956-984-6240Address: 1900 W. SchuniorCity: Edinburg</t>
+          <t>Proyecto Desarrollo Humano</t>
         </is>
       </c>
     </row>
@@ -2538,7 +2534,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Contact: DavidEmail: david@tsav.orgPhone: 1-956-364-2022Address: 1409 N. Stuart Place Rd., Suite DCity: Harlingen</t>
+          <t>Proyecto Juan Diego</t>
         </is>
       </c>
     </row>
@@ -2548,7 +2544,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Contact: Sylvia SepulvedaEmail: sylvia.sepulveda@co.hidalgo.tx.usPhone: 1-956-292-7000Address: 2524 N. Closner Blvd.City: Edinburg</t>
+          <t>Quinta Mazatlan World Birding Center</t>
         </is>
       </c>
     </row>
@@ -2558,7 +2554,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Contact: Juan LongoriaEmail: team@revjlo.orgPhone: 1-956-433-3738Address: 200 Menard DrCity: San Benito</t>
+          <t>Racks n Tusks</t>
         </is>
       </c>
     </row>
@@ -2568,7 +2564,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Contact: SonjaEmail: SonjaOrtega@aol.comPhone: 1-956-968-9030Address: 521 S Illinois AveCity: Weslaco</t>
+          <t>Raymondville Chamber of Commerce</t>
         </is>
       </c>
     </row>
@@ -2578,7 +2574,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Contact: Luzelma G. CanalesEmail: lcanales@cftexas.orgPhone: 1-956-225-5535Address: 407 N. 77 Sunshine StripCity: Harlingen</t>
+          <t>Recovery Center of Cameron County (RCCC, Inc.)</t>
         </is>
       </c>
     </row>
@@ -2588,7 +2584,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Contact: Dr. Norma L.Email: nsalaiz.rgvlead@gmail.comPhone: 1-956-364-4519Address: 1902 N Loop 499City: Harlingen</t>
+          <t>Region One ESC</t>
         </is>
       </c>
     </row>
@@ -2598,7 +2594,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Contact: RebecaEmail: rcg_mimi01@yahoo.comPhone: 1-956-246-2473Address: 20445 Mile 6 WCity: Edinburg</t>
+          <t>Regional Advisory Council on Trauma</t>
         </is>
       </c>
     </row>
@@ -2608,7 +2604,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Contact: FranciscoEmail: mano495@hotmail.comPhone: 1-956-878-4062Address: 4500 N 10th St Ste 315City: McAllen</t>
+          <t>Retired and Senior Volunteer Program (RSVP)</t>
         </is>
       </c>
     </row>
@@ -2618,7 +2614,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Contact: ReneEmail: rramirezn66@gmail.comPhone: 1-956-487-7278Address: 6844 E. Hwy 83City: Rio Grande City</t>
+          <t>Revjlo</t>
         </is>
       </c>
     </row>
@@ -2628,7 +2624,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Contact: Maria F. CoriaEmail: mfzavala@habitat-rgv.orgPhone: 1-956-686-7455Address: 412 W Ash Ave.City: McAllen</t>
+          <t>RGV First Christian Academy</t>
         </is>
       </c>
     </row>
@@ -2638,7 +2634,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Contact: Nancy RodriguezEmail: Nancy.Rodriguez1@HCAHealthcare.comPhone: 1-956-618-4402Address: 1809 S. CynthiaCity: McAllen</t>
+          <t>RGV FOCUS/Educate Texas</t>
         </is>
       </c>
     </row>
@@ -2648,7 +2644,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Contact: Margaret VillanuevaEmail: rgrhvolunteers@gmail.comPhone: 1-956-632-6154Address: 101 E. Ridge Rd.City: McAllen</t>
+          <t>RGV LEAD</t>
         </is>
       </c>
     </row>
@@ -2658,7 +2654,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Contact: Norma FriedrichEmail: volunteer@rgvbf.orgPhone: 1-361-676-6416Address: 311 E TylerCity: Harlingen</t>
+          <t>RGV Queens/Lovable Warrior</t>
         </is>
       </c>
     </row>
@@ -2668,7 +2664,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Contact: DianaEmail: dramirezrgvda@yahoo.comPhone: 1-956-782-1900Address: 420 S Closner BlvdCity: Edinburg</t>
+          <t>RGV Vipers Foundation</t>
         </is>
       </c>
     </row>
@@ -2678,7 +2674,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Contact: DaliaEmail: dalia@rgvez.orgPhone: 1-956-424-3276Address: 416 S Alton BlvdCity: Alton</t>
+          <t>Rio Grande City Consolidated School District Grulla High School</t>
         </is>
       </c>
     </row>
@@ -2688,7 +2684,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Contact: Diana FariasEmail: director@rgvliteracycenter.orgPhone: 1-956-961-4299Address: 1005 W Gore AvenueCity: Pharr</t>
+          <t>Rio Grande Habitat for Humanity</t>
         </is>
       </c>
     </row>
@@ -2698,7 +2694,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Contact: SergioEmail: Sergio@rgvpartnership.comPhone: 1-956-355-0011Address: 322 S Missouri AveCity: Weslaco</t>
+          <t>Rio Grande Regional Hospital Outpatient Surgery Center Volunteer Program</t>
         </is>
       </c>
     </row>
@@ -2708,7 +2704,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Contact: BrendaEmail: bsegovia@splch.comPhone: 1-408-512-8708Address: 602 Morgan Blvd.City: Harlingen</t>
+          <t>Rio Grande Regional Hospital Volunteer Auxiliary</t>
         </is>
       </c>
     </row>
@@ -2718,7 +2714,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Contact: Denise CantuEmail: dcantu@rmhcrgv.orgPhone: 1-956-412-7200Address: 1102 W. Trenton 3rd FloorCity: Edinburg</t>
+          <t>Rio Grande Valley Birding Festival</t>
         </is>
       </c>
     </row>
@@ -2728,7 +2724,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Contact: Denise CantuEmail: dcantu@rmhcrgv.orgPhone:1-956-412-7200Address: 1720 Treasure Hills BlvdCity: Harlingen</t>
+          <t>Rio Grande Valley Diabetes Association</t>
         </is>
       </c>
     </row>
@@ -2738,7 +2734,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Contact: Michael McNewEmail: mmcnew@mcallen.netPhone: 1-361-652-5766Address: 1300 Houston AvenueCity: McAllen</t>
+          <t>Rio Grande Valley Empowerment Zone</t>
         </is>
       </c>
     </row>
@@ -2748,7 +2744,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Contact: Pablo QuintanillaEmail: gsfinc@gmail.comPhone: 1-956-541-8034Address: 8435 Sabal Palm Rd.City: Brownsville</t>
+          <t>Rio Grande Valley Literacy Center</t>
         </is>
       </c>
     </row>
@@ -2758,7 +2754,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Contact: TeresaEmail: teresadejesus@sacredheartedinburg.orgPhone: 1-956-383-3253Address: 501 E KuhnCity: Edinburg</t>
+          <t>Rio Grande Valley Partnership</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2764,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Contact: Angela RidlingEmail: safehavenforkids@yahoo.comPhone: 1-956-515-5437Address: 1700 N. Alamo RdCity: Alamo</t>
+          <t>RioMAC</t>
         </is>
       </c>
     </row>
@@ -2778,7 +2774,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Contact: AliciaEmail: alicia.rodriguez@co.hidalgo.tx.usPhone: 1-956-387-0692Address: 230 N 86th StCity: Edinburg</t>
+          <t>Ronald McDonald Family Room</t>
         </is>
       </c>
     </row>
@@ -2788,7 +2784,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Contact: Kat LillieEmail: seaturtleinc@gmail.comPhone: 1-956-761-451Address: PO Box 3987City: South Padre Island</t>
+          <t>Ronald McDonald House Charities Rio Grande Valley</t>
         </is>
       </c>
     </row>
@@ -2798,7 +2794,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Contact: RickEmail: sebmud@aol.comPhone: 1-956-347-3036Address: 325 W 2nd StCity: Sebastian</t>
+          <t>Run Ride Share</t>
         </is>
       </c>
     </row>
@@ -2808,7 +2804,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Contact: MichelleEmail: michelle.zeager@utrgv.eduPhone: 1-956-296-1303</t>
+          <t>Sabal Palm Sanctuary</t>
         </is>
       </c>
     </row>
@@ -2818,7 +2814,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Contact: Javier GonzzalezzEmail: naturalist@spibirding.comPhone: 1-956-761-6801Address: 6801 Padre BoulevardCity: South Padre Island</t>
+          <t>Sacred Heart Parish</t>
         </is>
       </c>
     </row>
@@ -2828,7 +2824,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Contact: RoxanneEmail: roxanne@spichamber.comPhone: 1-956-761-4412Address: 610 Padre BlvdCity: South Padre Island</t>
+          <t>Safe Haven for Kids/Emergency Shelter</t>
         </is>
       </c>
     </row>
@@ -2838,7 +2834,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Contact: DennisEmail: dennis@frankerealty.comPhone: 1-956-761-0044Address: P.O. Box 2108City: South Padre Island</t>
+          <t>San Carlos Commuinty Resource Center</t>
         </is>
       </c>
     </row>
@@ -2848,7 +2844,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Contact: Emily SlyderEmail: volunteer@runspi.comPhone: 1-940-648-8900City: South Padre Island</t>
+          <t>Sea Turtle, Inc.</t>
         </is>
       </c>
     </row>
@@ -2858,7 +2854,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Contact: Juan GarciaEmail: staivargv@gmail.comPhone: 1-956-509-6355Address: 519 E Madison StCity: Brownsville</t>
+          <t>Sebastian Water Supply Corp.</t>
         </is>
       </c>
     </row>
@@ -2868,7 +2864,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Contact: AlmaEmail: amartinez@stchd.orgPhone: 1-956-797-2324Address: 108 S Main StCity: La Feria</t>
+          <t>SoM</t>
         </is>
       </c>
     </row>
@@ -2878,7 +2874,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Contact: MathewEmail: mshebbar@southtexascollege.eduPhone: 1-956-872-2147Address: Pecan Campus</t>
+          <t>South Padre Island Birding and Nature Center</t>
         </is>
       </c>
     </row>
@@ -2888,7 +2884,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Contact: Catalina RamosEmail: Sotxcta@gmail.comPhone: 1-956-874-4323Address: 618 N. McCollCity: McAllen</t>
+          <t>South Padre Island Chamber of Commerce</t>
         </is>
       </c>
     </row>
@@ -2898,7 +2894,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Contact: Debra FrancoEmail: dfranco@stjda.orgPhone: 1-956-627-5594Address: 313 W Nolana AveCity: McAllen</t>
+          <t>South Padre Island Community Foundation Inc</t>
         </is>
       </c>
     </row>
@@ -2908,7 +2904,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Contact: Denisse SadaEmail: stxliteracy@gmail.comPhone: 1-956-292-0257Address: 108 N. Jackson Rd.City: Edinburg</t>
+          <t>South Padre Marathon</t>
         </is>
       </c>
     </row>
@@ -2918,7 +2914,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Contact: GiselaEmail: gisela_chapa@fws.govPhone: 1-956-784-7541Address: 3325 Green Jay RoadCity: Alamo</t>
+          <t>South Texas Afghanistan Iraq Veterans Association</t>
         </is>
       </c>
     </row>
@@ -2928,7 +2924,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Contact: AngelicaEmail: stpa08@sbcglobal.netPhone: 1-956-460-9606Address: 413 Vista BonitaCity: Edinburg</t>
+          <t>South Texas Collaborative for Housing Development, Inc. (STCHD)</t>
         </is>
       </c>
     </row>
@@ -2938,7 +2934,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Contact: SuzanneEmail: admin@valleyorchestra.orgPhone: 1-956-661-1615Address: P.O. Box 2832City: McAllen</t>
+          <t>South Texas College</t>
         </is>
       </c>
     </row>
@@ -2948,7 +2944,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Contact: AngelicaEmail: sotxcta@gmail.comPhone: 1-956-821-3232Address:PO Box 668City: McAllen</t>
+          <t>South Texas Community Tennis Association</t>
         </is>
       </c>
     </row>
@@ -2958,7 +2954,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Contact: Petra de LeonEmail: pdeleon89@yahoo.comPhone: 1-956-546-7378Address: 440 E Ruben Torres BlvdCity: Brownsville</t>
+          <t>South Texas Juvenile Diabetes Association</t>
         </is>
       </c>
     </row>
@@ -2968,7 +2964,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Contact: Sandra GarzaEmail: sandy@scan-inc.orgPhone: 1-956-716-1795Address: Fort Ringgold Hwy 83City: Rio Grande City</t>
+          <t>South Texas Literacy Coalition</t>
         </is>
       </c>
     </row>
@@ -2978,7 +2974,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Contact: Nilda ElizondoEmail: nildaelizondo@starrcounty.orgPhone: 1-956-487-2709Address: 601 E. Main St.City: Rio Grande City</t>
+          <t>South Texas National Wildlife Refuge Complex</t>
         </is>
       </c>
     </row>
@@ -2988,7 +2984,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Contact: RhodaEmail: rreyes@startcenter.orgPhone: 1-956-399-7818Address: 743 North Sam HoustonCity: San Benito</t>
+          <t>South Texas Promotora Association</t>
         </is>
       </c>
     </row>
@@ -2998,7 +2994,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Contact: LauraEmail: gomez.laura@epa.govPhone: 1-956-578-1547City: Brownsville</t>
+          <t>South Texas Symphony Association Inc.</t>
         </is>
       </c>
     </row>
@@ -3008,7 +3004,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Contact: Belinda SimonsEmail: scde11@aol.comPhone: 1-956-781-0276Address: 8000 Cisne StreetCity: 1-956-781-0276</t>
+          <t>South Texas Community Tennis Association (CTA)</t>
         </is>
       </c>
     </row>
@@ -3018,7 +3014,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Contact: MariaEmail: mrenteria@suclinica.orgPhone: 1-956-365-6082Address: 1706 Treasure Hills BlvdCity: Harlingen</t>
+          <t>Spanish Meadows</t>
         </is>
       </c>
     </row>
@@ -3028,7 +3024,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Contact: Maria C. MercadoEmail: superrami25@hotmail.comPhone: 1-956-360-9982Address: 4112 Toronto AveCity: McAllen</t>
+          <t>Star County Community Coalition (SCAN)</t>
         </is>
       </c>
     </row>
@@ -3038,7 +3034,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Contact: NadiaEmail: nadia.m.kennedy.ctr@mail.milPhone: 1-956-724-6300 EXT#7464101Address: 6001 Bob Bullock LoopCity: Laredo</t>
+          <t>Starr County Historical Foundation</t>
         </is>
       </c>
     </row>
@@ -3048,7 +3044,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Contact: Sarai GarciaEmail: sgarcia@mcallen.netPhone: 1-956-681-3350Address: 1000 S. Ware RoadCity: McAllen</t>
+          <t>Start Center</t>
         </is>
       </c>
     </row>
@@ -3058,7 +3054,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Contact: Jonathan StevensEmail: Jonathan.Stevens@teachforamerica.orgPhone: 1-956-630-6781Address: 801 N. Bryan Rd.Suite 152City: Mission, TX 78572</t>
+          <t>Stronger Cities, Stronger Communities (SC2)</t>
         </is>
       </c>
     </row>
@@ -3068,7 +3064,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Su Casa De Esperanza, Inc.</t>
         </is>
       </c>
     </row>
@@ -3078,7 +3074,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Contact: Krystal GarciaEmail: info@teammario.orgPhone: 1-956-509-4121Address: PO Box 2985City: Edinburg</t>
+          <t>Su Clinica</t>
         </is>
       </c>
     </row>
@@ -3088,7 +3084,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Contact: Alma Elizabeth FloresEmail: lillyvalley7777@yahoo.comPhone: 1-956-929-4979Address: CantonCity: Edinburg</t>
+          <t>SuperRami and Friends INC</t>
         </is>
       </c>
     </row>
@@ -3098,7 +3094,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Contact: Ashley GregoryEmail: ahgregory@ag.tamu.eduPhone: 1-956-383-1026Address: 410 N. 13th Ave.City: Edinburg</t>
+          <t>Survivor Outreach Services for Military Families</t>
         </is>
       </c>
     </row>
@@ -3108,7 +3104,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Contact: Olga C.Email: gabriel@tamhsc.eduPhone: 1-956-668-6300Address: 2101 South McColll RdCity: McAllen</t>
+          <t>T.A.A.F. Summer Games of Texas – McAllen, Texas</t>
         </is>
       </c>
     </row>
@@ -3118,7 +3114,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Contact: Adela ArellanoEmail: aarellano@arch.tamu.eduPhone: 1-877-477-9355Address: 9355 3516 E EX 83City: Weslaco</t>
+          <t>Teach For America Rio Grande Valley</t>
         </is>
       </c>
     </row>
@@ -3128,7 +3124,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Contact: Myrna Irene TrevinoEmail: mtrevino@arch.tamu.eduPhone: 1-956-447-9355Address: 3516 E. Expressway 83City: Weslaco</t>
+          <t>Team Mario</t>
         </is>
       </c>
     </row>
@@ -3138,7 +3134,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Contact: LucillaEmail: lucilalagace@gmail.comPhone: 1-512-287-2043Address: 9011 Mountain Ridge DriveCity: Austin</t>
+          <t>Templo Biblico El Rey Ya Viene</t>
         </is>
       </c>
     </row>
@@ -3148,7 +3144,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Contact: Reynaldo AvilaEmail: reyavila@sbcglobal.netPhone: 1-956-245-1666Address: P.O. Box 1523City: San Benito</t>
+          <t>Texas A&amp;M AgriLife Extension – Deep South Texas Master Gardener Association</t>
         </is>
       </c>
     </row>
@@ -3158,7 +3154,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Contact: RoseEmail: rose.trevino@tdcj.texas.govPhone: 1-361-888-5698 ext. 201Address: 422 Sun Belt Dr.City: Corpus Christi</t>
+          <t>Texas A&amp;M Health Science Center</t>
         </is>
       </c>
     </row>
@@ -3168,7 +3164,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Contact: Debra FrancoEmail: debra_franco@baylor.eduPhone: 1-956-540-7329Address: 200 S. 10th StCity: McAllen</t>
+          <t>Texas A&amp;M Promotoras Project</t>
         </is>
       </c>
     </row>
@@ -3178,7 +3174,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Contact: Edwina P. GarzaEmail: egarza@txorgansharing.orgPhone: 1-956-630-0884Address: 1400 N. McColl Rd.City: McAllen</t>
+          <t>Texas A&amp;M University Colonias Program</t>
         </is>
       </c>
     </row>
@@ -3188,7 +3184,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Contact: MarleneEmail: MChavez@TRLA.ORGPhone: 1-956-447-4800Address: 301 S. TexasCity: Mercedes</t>
+          <t>Texas Association of Nonprofit Organizations (TANO)</t>
         </is>
       </c>
     </row>
@@ -3198,7 +3194,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Contact: BenEmail: benino.capetillo@tstc.eduPhone: 1-956-364-4023Address: 1902 North Loop 499City: Harlingen</t>
+          <t>Texas Conjunto Music Hall of Fame &amp; Museum</t>
         </is>
       </c>
     </row>
@@ -3208,7 +3204,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Contact: ChristopherEmail: crh153@txstate.eduPhone: 1-956-961-9749Address: 601 University DriveCity: San Marcos</t>
+          <t>Texas Crime Victims Clearinghouse TDCJ Victim Services Division</t>
         </is>
       </c>
     </row>
@@ -3218,7 +3214,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Contact: FernandoEmail: f.valle@ttu.eduPhone: 1-956-533-9676Address: 3008 18th St. EDUC 316City: Lubbock</t>
+          <t>Texas Hunger Initiative – Baylor University</t>
         </is>
       </c>
     </row>
@@ -3228,7 +3224,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Contact: GerardoEmail: gerardo.garza@tvc.texas.govPhone: 1-956-289-4542Address: 2719 W. UniversityCity: Edinburg</t>
+          <t>Texas Organ Sharing Alliance</t>
         </is>
       </c>
     </row>
@@ -3238,7 +3234,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Contact: PedroEmail: pedro.saldana@tvc.texas.govPhone: 1-956-443-4171City: Brownsville</t>
+          <t>Texas Rio Grande Legal Aid Inc (TRLA)</t>
         </is>
       </c>
     </row>
@@ -3248,7 +3244,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Contact: Leigh AnnEmail: leighann.godinez@twc.state.tx.usPhone: 1-956-212-5188Address: 3101 W. Business 83City: McAllen</t>
+          <t>Texas State Technical College (TSTC)</t>
         </is>
       </c>
     </row>
@@ -3258,7 +3254,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Contact: Gilberto Jr.Email: tmbc@tm-bc.orgPhone: 1-956-481-3256Address: P.O. Box 127City: San Isidro</t>
+          <t>Texas State University</t>
         </is>
       </c>
     </row>
@@ -3268,7 +3264,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Contact: Roger Astudillo</t>
+          <t>Texas Tech University, College of Education</t>
         </is>
       </c>
     </row>
@@ -3278,7 +3274,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Email: rogelio.astudillo@co.hidalgo.tx.usPhone: 1-956-283-1711Address: 1429 S Tower RoadCity: Alamo</t>
+          <t>Texas Veterans Commission</t>
         </is>
       </c>
     </row>
@@ -3288,7 +3284,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Contact: DebbieEmail: debbie.tpcc@gmail.comPhone: 1-956-263-1387Address: 214 Chaparral BlvdCity: Rio Grande City</t>
+          <t>Texas Workforce Commission Project HIRE (Helping Individuals Reach Employment)</t>
         </is>
       </c>
     </row>
@@ -3298,7 +3294,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Contact: LarryEmail: larrywilson1950@gmail.comPhone: 1-956-631-0612Address: 301 Shasta AveCity: McAllen</t>
+          <t>Texas/Mexico Border Coalition Community Based Org.</t>
         </is>
       </c>
     </row>
@@ -3308,7 +3304,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Contact: MariaEmail: info@lrgvaia.orgEmail: msustaeta@lrgvaia.orgPhone: 1-956-994-0939Address: 302 South Texas Ave.City: Mercedes</t>
+          <t>The Alamo Community Resource Center</t>
         </is>
       </c>
     </row>
@@ -3318,7 +3314,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Contact: SandraEmail: ssanchez@themonitor.comPhone: 1-956-605-0470Address: 400 E Nolana AveCity: McAllen</t>
+          <t>The Child Wellness Network, INC</t>
         </is>
       </c>
     </row>
@@ -3328,7 +3324,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Contact: Sadie MaciasEmail: sadie.macias@uss.salvationarmy.orgPhone: 1-956-682-1468Address: 1600 N. 23rd St.City: McAllen</t>
+          <t>The Church of Jesus Christ of Latter Day Saints</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3334,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Contact: Marcos SilvaEmail: Michael@stxideas.comPhone: 1-956-739-0606Address: 14001 Rooth RdCity: Edinburg</t>
+          <t>The Lower Rio Grande Valley Chapter of the American Institute of Architecture</t>
         </is>
       </c>
     </row>
@@ -3348,7 +3344,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Contact: ArleneEmail: arlene.laboy01@utrgv.eduPhone: 1-956-314-1348Address: 1 W. University BlvdCity: Brownsville</t>
+          <t>The Monitor</t>
         </is>
       </c>
     </row>
@@ -3358,7 +3354,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Contact: Sara WalkerEmail: director@weslacomuseum.orgPhone: 1-956-968-9142Address: 500 S. Texas BoulevardCity: Weslaco</t>
+          <t>The Salvation Army – Hidalgo County</t>
         </is>
       </c>
     </row>
@@ -3368,7 +3364,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Contact: Alma HerreraEmail: almaherrera.familyoutreach@yahoo.comPhone: 1-956-541-5566Address: 455 E. Levee St.City: Brownsville</t>
+          <t>The South Texas Ideas Festival (STXi)</t>
         </is>
       </c>
     </row>
@@ -3378,7 +3374,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Contact: JeaneEmail: Jeanemgarza@yahoo.comPhone: 1-956-369-6242Address: PO Box 2898City: Edinburg</t>
+          <t>The University of Texas Rio Grande Valley</t>
         </is>
       </c>
     </row>
@@ -3388,7 +3384,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Contact: Eric MastenEmail: emasten@bhsst.orgPhone: 1-956-787-0004Address: 5510 N Cage BlvdCity: Pharr</t>
+          <t>The Weslaco Museum</t>
         </is>
       </c>
     </row>
@@ -3398,7 +3394,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Contact: CesarEmail: merccado@outlook.comPhone: 1-956-832-9008Address: 1995 billy mitchell blvdCity: Brownsville</t>
+          <t>Tip of Texas Family Outreach</t>
         </is>
       </c>
     </row>
@@ -3408,7 +3404,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Contact: Mary AnnEmail: seafoxsea@sbcglobal.netPhone: 1-956-761-4002Address: 5805 Gulf BlvdCity: South Padre Island</t>
+          <t>To Sarah with Love</t>
         </is>
       </c>
     </row>
@@ -3418,7 +3414,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Contact: Christine DonaldEmail: Christine_Donald@fws.govPhone: 1-956-784-7575Address: 3325 Green Jay RoadCity: Alamo</t>
+          <t>Tobacco Prevention and Control Coalition</t>
         </is>
       </c>
     </row>
@@ -3428,7 +3424,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Contact: Thomas HasenauerEmail: LRGVDO.email@sba.govPhone: 1-956-427-8533Address: 2422 E. Tyler St.City: Harlingen</t>
+          <t>Trico Products</t>
         </is>
       </c>
     </row>
@@ -3438,7 +3434,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Contact: AngelaEmail: angela.burton@sba.govPhone: 1-956-427-8533Address: 2422 E Tyler AveCity: Harlingen</t>
+          <t>Turtle Lady Legacy</t>
         </is>
       </c>
     </row>
@@ -3448,7 +3444,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Contact: Frank EsparzaEmail: fesparza@bloodsystems.orgPhone: 1-956-213-7523Address: 1400 S. 6th StreetCity: McAllen</t>
+          <t>U.S. Fish &amp; Wildlife/South Texas Refuges</t>
         </is>
       </c>
     </row>
@@ -3458,7 +3454,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Contact: JessicaEmail: unitedwayncc@yahoo.comPhone: 1-956-423-5954Address: 134 E Van Buren Ave # ACity: Harlingen</t>
+          <t>U.S. Small Business Administration</t>
         </is>
       </c>
     </row>
@@ -3468,7 +3464,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Contact: Eloise MontemayorEmail: emontemayor@unitedwayofsotx.orgPhone: 1-956-686-6331Address: 113 W. Pecan Blvd.City: McAllen</t>
+          <t>United Blood Services</t>
         </is>
       </c>
     </row>
@@ -3478,7 +3474,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Contact: Wendy De LeonEmail: wendy.deleon@unitedwayrgv.orgPhone: 1-956-548-6880Address: 634 East Levee St.City: Brownsville</t>
+          <t>United Way of Northern Cameron County</t>
         </is>
       </c>
     </row>
@@ -3488,7 +3484,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Contact: Dora AlaffaEmail: Dora.Alaffa@upbring.orgPhone: 1-956-378-3070Address: 4616 N D StCity: Mcallen</t>
+          <t>United Way of South Texas</t>
         </is>
       </c>
     </row>
@@ -3498,7 +3494,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Contact: Wally CantuEmail: wcantu@valleyaids.orgPhone: 1-956-428-2653Address: 2306 Camelot Plaza CircleCity: Harlingen</t>
+          <t>United Way of Southern Cameron County</t>
         </is>
       </c>
     </row>
@@ -3508,7 +3504,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Contact: VeronicaEmail: veronica@vamosscholars.orgPhone: 1-956-800-4085Address: 800 N. Main Street Suite 410City: McAllen</t>
+          <t>Upbring</t>
         </is>
       </c>
     </row>
@@ -3518,7 +3514,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Contact: AnaEmail: vamospc@vamosscholars.orgPhone: 1-956-631-1273Address: 1-956-631-1273City: McAllen</t>
+          <t>Valley AIDS Council</t>
         </is>
       </c>
     </row>
@@ -3528,7 +3524,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Contact: ArturoEmail: turorodz@gmail.comPhone: 1-956-373-8199Address: 3016 N McColl Rd Suite BCity: Mcallen</t>
+          <t>Valley Alliance of Mentors for Opportunities and Scholarships (VAMOS)</t>
         </is>
       </c>
     </row>
@@ -3538,7 +3534,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Contact: Kristen MillonEmail: valleyhaveninc@gmail.comPhone: 1-956-893-0422Address: 5501 W Business 83City: Harlingen</t>
+          <t>Valley Association for Independent Living (V.A.I.L.)</t>
         </is>
       </c>
     </row>
@@ -3548,7 +3544,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Contact: Hollie JohnstonEmail: info@valleynaturecenter.orgPhone: 1-956-969-2475Address: 301 S. Border AvenueCity: Weslaco</t>
+          <t>Valley Haven Inc</t>
         </is>
       </c>
     </row>
@@ -3558,7 +3554,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Contact: Laura MaxwellEmail: vpec@valleyproud.orgPhone: 1-956-412-8004Address: 513 E. Jackson StreetCity: Harlingen</t>
+          <t>Valley Nature Center</t>
         </is>
       </c>
     </row>
@@ -3568,7 +3564,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Contact: VivianEmail: vivian@valleyorchestra.orgPhone: 1-956-661-1615Address: 200 S 10th St #104City: McAllen</t>
+          <t>Valley Proud Environmental Council</t>
         </is>
       </c>
     </row>
@@ -3578,7 +3574,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Contact: Laura MartinezEmail: lmilgun@vanniecook.orgPhone: 1-956-687-5146Address: 101 W. Expressway 83City: McAllen</t>
+          <t>Valley Symphony Orchestra</t>
         </is>
       </c>
     </row>
@@ -3588,7 +3584,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Contact: Arlene LaboyEmail: veteranfemalesunited@gmail.comPhone: 1-956-314-1348Address: P.O. Box 5481City: Brownsville</t>
+          <t>Vannie E Cook Jr. Childrens Cancer &amp; Hematology Clinic</t>
         </is>
       </c>
     </row>
@@ -3598,127 +3594,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Contact: Irma GarciaEmail: igarcia@vidacareers.orgPhone: 1-956-903-1900Address: 417 S OhioCity: Mercedes</t>
-        </is>
-      </c>
-    </row>
-    <row r="318">
-      <c r="A318" s="1" t="n">
-        <v>316</v>
-      </c>
-      <c r="B318" t="inlineStr">
-        <is>
-          <t>Contact: Keren AristaEmail: keren.arista@unitedwayrgv.orgPhone: 1-956-548-6880Address: 634 E. Levee St.City: Brownsville</t>
-        </is>
-      </c>
-    </row>
-    <row r="319">
-      <c r="A319" s="1" t="n">
-        <v>317</v>
-      </c>
-      <c r="B319" t="inlineStr">
-        <is>
-          <t>Contact: NancyEmail: nancy@wefna.orgEmail: mrs.nancy.rocha@gmail.comPhone: 1-956-878-6400Address: 412 W. Westway Ave. Mcallen, TXAddress: 78501 &amp; 1201 W University Dr HP1 1.110-G, Edinburg, TXCity: Mcallen &amp; Edinburg</t>
-        </is>
-      </c>
-    </row>
-    <row r="320">
-      <c r="A320" s="1" t="n">
-        <v>318</v>
-      </c>
-      <c r="B320" t="inlineStr">
-        <is>
-          <t>Contact: Nelda HernandezEmail: nhernandezfjc@yahoo.comPhone: 1-956-630-4878Address: 511 N. Cynthia StreetCity: McAllen</t>
-        </is>
-      </c>
-    </row>
-    <row r="321">
-      <c r="A321" s="1" t="n">
-        <v>319</v>
-      </c>
-      <c r="B321" t="inlineStr">
-        <is>
-          <t>Contact: Andrea BentonEmail: andrea@wbc-cc.comPhone: 1-956-542-5322Address: 1600 W. University Blvd.City: Brownsville</t>
-        </is>
-      </c>
-    </row>
-    <row r="322">
-      <c r="A322" s="1" t="n">
-        <v>320</v>
-      </c>
-      <c r="B322" t="inlineStr">
-        <is>
-          <t>Contact: Francisco AlmarazEmail: francisco@wfsolutions.orgPhone: 1-956-928-5000Address: 3101 W. Business 83City: McAllen</t>
-        </is>
-      </c>
-    </row>
-    <row r="323">
-      <c r="A323" s="1" t="n">
-        <v>321</v>
-      </c>
-      <c r="B323" t="inlineStr">
-        <is>
-          <t>Contact: Marisa Almaraz (Executive Assistant/Travel Coordinator)Email: marisa.almaraz@wfscameron.orgPhone: 956.548.6700Address:700 Ruben M. Torres Blvd., 3rd Floor, Brownsville, Texas 78520</t>
-        </is>
-      </c>
-    </row>
-    <row r="324">
-      <c r="A324" s="1" t="n">
-        <v>322</v>
-      </c>
-      <c r="B324" t="inlineStr">
-        <is>
-          <t>Contact: Christopher SotoEmail: Info@yaquianimalrescue.comPhone: 1-956-651-8636Address: 500 Venecia Dr.City: Sullivan City</t>
-        </is>
-      </c>
-    </row>
-    <row r="325">
-      <c r="A325" s="1" t="n">
-        <v>323</v>
-      </c>
-      <c r="B325" t="inlineStr">
-        <is>
-          <t>Contact: Janeth RicoEmail: jrico@cdcb.orgPhone: 1-956-548-2302Address: 815 Arthur StCity: Brownsville</t>
-        </is>
-      </c>
-    </row>
-    <row r="326">
-      <c r="A326" s="1" t="n">
-        <v>324</v>
-      </c>
-      <c r="B326" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The RGV Partnership is composed of community-minded business leaders that are devoted to successfully promote community growth to our business entities within the four-county region. </t>
-        </is>
-      </c>
-    </row>
-    <row r="327">
-      <c r="A327" s="1" t="n">
-        <v>325</v>
-      </c>
-      <c r="B327" t="inlineStr">
-        <is>
-          <t>Address:322 S Missouri Ave., Weslaco TX 78596</t>
-        </is>
-      </c>
-    </row>
-    <row r="328">
-      <c r="A328" s="1" t="n">
-        <v>326</v>
-      </c>
-      <c r="B328" t="inlineStr">
-        <is>
-          <t>Phone: 956.968.3141</t>
-        </is>
-      </c>
-    </row>
-    <row r="329">
-      <c r="A329" s="1" t="n">
-        <v>327</v>
-      </c>
-      <c r="B329" t="inlineStr">
-        <is>
-          <t>Email: info@rgvpartnership.com</t>
+          <t>Veteran Females United</t>
         </is>
       </c>
     </row>

</xml_diff>